<commit_message>
finalizei paineis do desfecho, falta juntar
</commit_message>
<xml_diff>
--- a/res/treat_dur_stat_cam.xlsx
+++ b/res/treat_dur_stat_cam.xlsx
@@ -1,110 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufscbr-my.sharepoint.com/personal/tamires_martins_ufsc_br/Documents/PC LAB/DissAnalysis/res/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_6F68FDCE8F79A8D366075C52F3F392B399BEFEC8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
-  <si>
-    <t>skim_type</t>
-  </si>
-  <si>
-    <t>skim_variable</t>
-  </si>
-  <si>
-    <t>treatment_via</t>
-  </si>
-  <si>
-    <t>complete</t>
-  </si>
-  <si>
-    <t>numeric.mean</t>
-  </si>
-  <si>
-    <t>numeric.sd</t>
-  </si>
-  <si>
-    <t>numeric.p0</t>
-  </si>
-  <si>
-    <t>numeric.p25</t>
-  </si>
-  <si>
-    <t>numeric.p50</t>
-  </si>
-  <si>
-    <t>numeric.p75</t>
-  </si>
-  <si>
-    <t>numeric.p100</t>
-  </si>
-  <si>
-    <t>numeric.hist</t>
-  </si>
-  <si>
-    <t>numeric.median</t>
-  </si>
-  <si>
-    <t>numeric.iqr</t>
-  </si>
-  <si>
-    <t>numeric</t>
-  </si>
-  <si>
-    <t>treatment_duration</t>
-  </si>
-  <si>
-    <t>Gavagem</t>
-  </si>
-  <si>
-    <t>▇▃▁▂▂</t>
-  </si>
-  <si>
-    <t>Intraperitoneal</t>
-  </si>
-  <si>
-    <t>▇▁▁▁▁</t>
-  </si>
-  <si>
-    <t>Sem info</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Oral</t>
-  </si>
-  <si>
-    <t>▇▂▁▁▁</t>
-  </si>
-  <si>
-    <t>Subcutânea</t>
-  </si>
-  <si>
-    <t>▇▁▁▁▃</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,19 +63,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -206,7 +109,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -238,27 +141,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -290,24 +175,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -483,68 +350,100 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>skim_type</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>skim_variable</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>treatment_via</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>complete</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>numeric.mean</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>numeric.sd</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>numeric.p0</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>numeric.p25</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>numeric.p50</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>numeric.p75</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>numeric.p100</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>numeric.hist</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>numeric.median</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>numeric.iqr</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>numeric</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>treatment_duration</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Gavagem</t>
+        </is>
       </c>
       <c r="D2">
         <v>24</v>
@@ -553,7 +452,7 @@
         <v>6.666666666666667</v>
       </c>
       <c r="F2">
-        <v>7.1180521680208741</v>
+        <v>7.118052168020874</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -570,8 +469,10 @@
       <c r="K2">
         <v>21</v>
       </c>
-      <c r="L2" t="s">
-        <v>17</v>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>▇▃▁▂▂</t>
+        </is>
       </c>
       <c r="M2">
         <v>4</v>
@@ -580,21 +481,27 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>numeric</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>treatment_duration</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Intraperitoneal</t>
+        </is>
       </c>
       <c r="D3">
         <v>206</v>
       </c>
       <c r="E3">
-        <v>3.2572815533980579</v>
+        <v>3.257281553398058</v>
       </c>
       <c r="F3">
         <v>11.82501772858361</v>
@@ -614,8 +521,10 @@
       <c r="K3">
         <v>110</v>
       </c>
-      <c r="L3" t="s">
-        <v>19</v>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>▇▁▁▁▁</t>
+        </is>
       </c>
       <c r="M3">
         <v>1</v>
@@ -624,41 +533,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>numeric</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>treatment_duration</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Sem info</t>
+        </is>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="L4" t="s">
-        <v>21</v>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>numeric</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>treatment_duration</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Oral</t>
+        </is>
       </c>
       <c r="D5">
         <v>76</v>
       </c>
       <c r="E5">
-        <v>14.763157894736841</v>
+        <v>14.76315789473684</v>
       </c>
       <c r="F5">
-        <v>21.247034880850322</v>
+        <v>21.24703488085032</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -675,8 +598,10 @@
       <c r="K5">
         <v>90</v>
       </c>
-      <c r="L5" t="s">
-        <v>23</v>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>▇▂▁▁▁</t>
+        </is>
       </c>
       <c r="M5">
         <v>7</v>
@@ -685,24 +610,30 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>numeric</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>treatment_duration</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Subcutânea</t>
+        </is>
       </c>
       <c r="D6">
         <v>14</v>
       </c>
       <c r="E6">
-        <v>4.4285714285714288</v>
+        <v>4.428571428571429</v>
       </c>
       <c r="F6">
-        <v>5.6256867712619449</v>
+        <v>5.625686771261945</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -719,8 +650,10 @@
       <c r="K6">
         <v>13</v>
       </c>
-      <c r="L6" t="s">
-        <v>25</v>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>▇▁▁▁▃</t>
+        </is>
       </c>
       <c r="M6">
         <v>1</v>

</xml_diff>